<commit_message>
Generated the outputs to show the stakeholders to start the conversation for CDC project
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/composition-otherdiagreport-1.xlsx
+++ b/output/DiagnosticReport/composition-otherdiagreport-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="473">
   <si>
     <t>Path</t>
   </si>
@@ -619,7 +619,7 @@
 </t>
   </si>
   <si>
-    <t>Kind of composition (LOINC if possible)</t>
+    <t>Document sub-type, also referred to as document category</t>
   </si>
   <si>
     <t>Specifies the particular kind of composition (e.g. History and Physical, Discharge Summary, Progress Note). This usually equates to the purpose of making the composition.</t>
@@ -631,6 +631,14 @@
     <t>Key metadata element describing the composition, used in searching/filtering.</t>
   </si>
   <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://loinc.org"/&gt;
+    &lt;code value="47045-0"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
     <t>Type of a composition.</t>
   </si>
   <si>
@@ -655,7 +663,7 @@
     <t>Composition.category</t>
   </si>
   <si>
-    <t>Categorization of Composition</t>
+    <t>Document type</t>
   </si>
   <si>
     <t>A categorization for the type of the composition - helps for indexing and searching. This may be implied by or derived from the code specified in the Composition Type.</t>
@@ -4128,7 +4136,7 @@
         <v>41</v>
       </c>
       <c r="R22" t="s" s="2">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>41</v>
@@ -4146,10 +4154,10 @@
         <v>135</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>41</v>
@@ -4182,24 +4190,24 @@
         <v>88</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4207,13 +4215,13 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>41</v>
@@ -4225,16 +4233,16 @@
         <v>191</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -4262,10 +4270,10 @@
         <v>120</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>41</v>
@@ -4283,7 +4291,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
@@ -4298,24 +4306,24 @@
         <v>88</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>70</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4338,19 +4346,19 @@
         <v>54</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>41</v>
@@ -4399,7 +4407,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>42</v>
@@ -4417,21 +4425,21 @@
         <v>41</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4454,17 +4462,17 @@
         <v>54</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>41</v>
@@ -4513,7 +4521,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>42</v>
@@ -4528,24 +4536,24 @@
         <v>88</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4568,19 +4576,19 @@
         <v>54</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>41</v>
@@ -4629,7 +4637,7 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>53</v>
@@ -4644,24 +4652,24 @@
         <v>88</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4672,7 +4680,7 @@
         <v>53</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>54</v>
@@ -4684,17 +4692,17 @@
         <v>54</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>41</v>
@@ -4743,7 +4751,7 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>53</v>
@@ -4758,24 +4766,24 @@
         <v>88</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4801,13 +4809,13 @@
         <v>55</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4857,7 +4865,7 @@
         <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>53</v>
@@ -4875,13 +4883,13 @@
         <v>41</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>41</v>
@@ -4889,7 +4897,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4915,13 +4923,13 @@
         <v>130</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4950,10 +4958,10 @@
         <v>184</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>41</v>
@@ -4971,7 +4979,7 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4989,13 +4997,13 @@
         <v>41</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>41</v>
@@ -5003,7 +5011,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5026,19 +5034,19 @@
         <v>41</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>41</v>
@@ -5087,7 +5095,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -5099,19 +5107,19 @@
         <v>41</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>41</v>
@@ -5119,7 +5127,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5231,7 +5239,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5345,11 +5353,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -5371,10 +5379,10 @@
         <v>73</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>76</v>
@@ -5429,7 +5437,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>42</v>
@@ -5461,7 +5469,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5487,21 +5495,21 @@
         <v>130</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P34" s="2"/>
       <c r="Q34" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="R34" t="s" s="2">
         <v>41</v>
@@ -5522,10 +5530,10 @@
         <v>184</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>41</v>
@@ -5543,7 +5551,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>53</v>
@@ -5561,10 +5569,10 @@
         <v>41</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>41</v>
@@ -5575,7 +5583,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5598,17 +5606,17 @@
         <v>41</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>41</v>
@@ -5657,7 +5665,7 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5675,10 +5683,10 @@
         <v>41</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>41</v>
@@ -5689,7 +5697,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5712,17 +5720,17 @@
         <v>41</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>41</v>
@@ -5771,7 +5779,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>42</v>
@@ -5789,21 +5797,21 @@
         <v>41</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5826,19 +5834,19 @@
         <v>54</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>41</v>
@@ -5887,7 +5895,7 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>42</v>
@@ -5905,13 +5913,13 @@
         <v>41</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>41</v>
@@ -5919,7 +5927,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5942,16 +5950,16 @@
         <v>41</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -6001,7 +6009,7 @@
         <v>41</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
@@ -6019,13 +6027,13 @@
         <v>41</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>41</v>
@@ -6033,7 +6041,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6145,7 +6153,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6259,11 +6267,11 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
@@ -6285,10 +6293,10 @@
         <v>73</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M41" t="s" s="2">
         <v>76</v>
@@ -6343,7 +6351,7 @@
         <v>41</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>42</v>
@@ -6375,7 +6383,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6401,13 +6409,13 @@
         <v>130</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6436,10 +6444,10 @@
         <v>184</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>41</v>
@@ -6457,7 +6465,7 @@
         <v>41</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>53</v>
@@ -6475,13 +6483,13 @@
         <v>41</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>41</v>
@@ -6489,7 +6497,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6512,13 +6520,13 @@
         <v>41</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6569,7 +6577,7 @@
         <v>41</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>53</v>
@@ -6587,13 +6595,13 @@
         <v>41</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>41</v>
@@ -6601,7 +6609,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6624,19 +6632,19 @@
         <v>54</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>41</v>
@@ -6685,7 +6693,7 @@
         <v>41</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>42</v>
@@ -6703,13 +6711,13 @@
         <v>41</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>41</v>
@@ -6717,7 +6725,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6829,7 +6837,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6943,11 +6951,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6969,10 +6977,10 @@
         <v>73</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>76</v>
@@ -7027,7 +7035,7 @@
         <v>41</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>42</v>
@@ -7059,7 +7067,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7085,13 +7093,13 @@
         <v>191</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -7120,10 +7128,10 @@
         <v>120</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>41</v>
@@ -7141,7 +7149,7 @@
         <v>41</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>42</v>
@@ -7159,13 +7167,13 @@
         <v>41</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>41</v>
@@ -7173,7 +7181,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7196,13 +7204,13 @@
         <v>54</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7253,7 +7261,7 @@
         <v>41</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>42</v>
@@ -7271,13 +7279,13 @@
         <v>41</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>41</v>
@@ -7285,7 +7293,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7308,13 +7316,13 @@
         <v>54</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7365,7 +7373,7 @@
         <v>41</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>42</v>
@@ -7383,7 +7391,7 @@
         <v>41</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>70</v>
@@ -7397,7 +7405,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7420,13 +7428,13 @@
         <v>41</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7477,7 +7485,7 @@
         <v>41</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>42</v>
@@ -7489,16 +7497,16 @@
         <v>41</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>41</v>
@@ -7509,7 +7517,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7621,7 +7629,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7735,11 +7743,11 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -7761,10 +7769,10 @@
         <v>73</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>76</v>
@@ -7819,7 +7827,7 @@
         <v>41</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>42</v>
@@ -7851,11 +7859,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7877,16 +7885,16 @@
         <v>55</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>41</v>
@@ -7935,7 +7943,7 @@
         <v>41</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>42</v>
@@ -7953,10 +7961,10 @@
         <v>41</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>41</v>
@@ -7967,7 +7975,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7993,16 +8001,16 @@
         <v>191</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>41</v>
@@ -8012,7 +8020,7 @@
         <v>41</v>
       </c>
       <c r="R56" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>41</v>
@@ -8030,10 +8038,10 @@
         <v>120</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>41</v>
@@ -8051,7 +8059,7 @@
         <v>41</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>42</v>
@@ -8069,10 +8077,10 @@
         <v>41</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>41</v>
@@ -8083,7 +8091,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8106,17 +8114,17 @@
         <v>41</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>41</v>
@@ -8165,7 +8173,7 @@
         <v>41</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -8183,21 +8191,21 @@
         <v>41</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8220,16 +8228,16 @@
         <v>41</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -8279,7 +8287,7 @@
         <v>41</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>42</v>
@@ -8300,7 +8308,7 @@
         <v>41</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>41</v>
@@ -8311,7 +8319,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8337,13 +8345,13 @@
         <v>141</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -8393,7 +8401,7 @@
         <v>41</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>42</v>
@@ -8402,7 +8410,7 @@
         <v>53</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>88</v>
@@ -8411,10 +8419,10 @@
         <v>41</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>41</v>
@@ -8425,7 +8433,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8451,23 +8459,23 @@
         <v>130</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P60" s="2"/>
       <c r="Q60" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="R60" t="s" s="2">
         <v>41</v>
@@ -8488,10 +8496,10 @@
         <v>184</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>41</v>
@@ -8509,7 +8517,7 @@
         <v>41</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8527,7 +8535,7 @@
         <v>41</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>70</v>
@@ -8536,12 +8544,12 @@
         <v>41</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8567,16 +8575,16 @@
         <v>191</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>41</v>
@@ -8604,10 +8612,10 @@
         <v>135</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>41</v>
@@ -8625,7 +8633,7 @@
         <v>41</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8643,7 +8651,7 @@
         <v>41</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>70</v>
@@ -8657,7 +8665,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8680,16 +8688,16 @@
         <v>41</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="K62" t="s" s="2">
         <v>44</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8739,7 +8747,7 @@
         <v>41</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>42</v>
@@ -8748,7 +8756,7 @@
         <v>43</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>88</v>
@@ -8757,10 +8765,10 @@
         <v>41</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>41</v>
@@ -8771,7 +8779,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8883,7 +8891,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8997,7 +9005,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9023,13 +9031,13 @@
         <v>55</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -9079,7 +9087,7 @@
         <v>41</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>42</v>
@@ -9088,7 +9096,7 @@
         <v>53</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>88</v>
@@ -9111,7 +9119,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9137,13 +9145,13 @@
         <v>96</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9172,10 +9180,10 @@
         <v>112</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>41</v>
@@ -9193,7 +9201,7 @@
         <v>41</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>42</v>
@@ -9225,7 +9233,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9251,13 +9259,13 @@
         <v>170</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9307,7 +9315,7 @@
         <v>41</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>42</v>
@@ -9325,7 +9333,7 @@
         <v>41</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>41</v>
@@ -9339,7 +9347,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9365,13 +9373,13 @@
         <v>55</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -9421,7 +9429,7 @@
         <v>41</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>42</v>
@@ -9453,7 +9461,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9479,16 +9487,16 @@
         <v>191</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>41</v>
@@ -9516,10 +9524,10 @@
         <v>135</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="Y69" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="Z69" t="s" s="2">
         <v>41</v>
@@ -9537,7 +9545,7 @@
         <v>41</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>42</v>
@@ -9546,7 +9554,7 @@
         <v>53</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>88</v>
@@ -9555,7 +9563,7 @@
         <v>41</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>70</v>
@@ -9569,7 +9577,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9595,13 +9603,13 @@
         <v>41</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -9651,7 +9659,7 @@
         <v>41</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>42</v>
@@ -9660,7 +9668,7 @@
         <v>43</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>88</v>
@@ -9669,10 +9677,10 @@
         <v>41</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
Composition Other Diagnostic report - moved fixed pattern to category
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/composition-otherdiagreport-1.xlsx
+++ b/output/DiagnosticReport/composition-otherdiagreport-1.xlsx
@@ -631,48 +631,48 @@
     <t>Key metadata element describing the composition, used in searching/filtering.</t>
   </si>
   <si>
+    <t>Type of a composition.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/doc-typecodes</t>
+  </si>
+  <si>
+    <t>Event.code</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>.code</t>
+  </si>
+  <si>
+    <t>DocumentReference.type</t>
+  </si>
+  <si>
+    <t>FiveWs.class</t>
+  </si>
+  <si>
+    <t>Composition.category</t>
+  </si>
+  <si>
+    <t>Document type</t>
+  </si>
+  <si>
+    <t>A categorization for the type of the composition - helps for indexing and searching. This may be implied by or derived from the code specified in the Composition Type.</t>
+  </si>
+  <si>
+    <t>This is a metadata field from [XDS/MHD](http://wiki.ihe.net/index.php?title=Mobile_access_to_Health_Documents_(MHD)).</t>
+  </si>
+  <si>
+    <t>Helps humans to assess whether the composition is of interest when viewing an index of compositions or documents.</t>
+  </si>
+  <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
     &lt;system value="http://loinc.org"/&gt;
     &lt;code value="47045-0"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>Type of a composition.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/doc-typecodes</t>
-  </si>
-  <si>
-    <t>Event.code</t>
-  </si>
-  <si>
-    <t>./code</t>
-  </si>
-  <si>
-    <t>.code</t>
-  </si>
-  <si>
-    <t>DocumentReference.type</t>
-  </si>
-  <si>
-    <t>FiveWs.class</t>
-  </si>
-  <si>
-    <t>Composition.category</t>
-  </si>
-  <si>
-    <t>Document type</t>
-  </si>
-  <si>
-    <t>A categorization for the type of the composition - helps for indexing and searching. This may be implied by or derived from the code specified in the Composition Type.</t>
-  </si>
-  <si>
-    <t>This is a metadata field from [XDS/MHD](http://wiki.ihe.net/index.php?title=Mobile_access_to_Health_Documents_(MHD)).</t>
-  </si>
-  <si>
-    <t>Helps humans to assess whether the composition is of interest when viewing an index of compositions or documents.</t>
   </si>
   <si>
     <t>High-level kind of a clinical document at a macro level.</t>
@@ -4136,7 +4136,7 @@
         <v>41</v>
       </c>
       <c r="R22" t="s" s="2">
-        <v>196</v>
+        <v>41</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>41</v>
@@ -4154,10 +4154,10 @@
         <v>135</v>
       </c>
       <c r="X22" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="Y22" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="Y22" t="s" s="2">
-        <v>198</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>41</v>
@@ -4190,24 +4190,24 @@
         <v>88</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>203</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4233,16 +4233,16 @@
         <v>191</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>207</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>208</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -4252,7 +4252,7 @@
         <v>41</v>
       </c>
       <c r="R23" t="s" s="2">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="S23" t="s" s="2">
         <v>41</v>
@@ -4291,7 +4291,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
@@ -4318,7 +4318,7 @@
         <v>213</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24">
@@ -7167,10 +7167,10 @@
         <v>41</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>361</v>
@@ -8077,10 +8077,10 @@
         <v>41</v>
       </c>
       <c r="AK56" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="AL56" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>41</v>
@@ -8544,7 +8544,7 @@
         <v>41</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" hidden="true">

</xml_diff>